<commit_message>
done part 1 of e1
</commit_message>
<xml_diff>
--- a/IIB/4A4/exercise1/exercise1data_2024.xlsx
+++ b/IIB/4A4/exercise1/exercise1data_2024.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28324"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://universityofcambridgecloud-my.sharepoint.com/personal/mv234_cam_ac_uk/Documents/Documents/1_4A4/2024-25/Coursework/2024/Exercise1/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\louis\source\repos\MEng-CW\IIB\4A4\exercise1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="7" documentId="13_ncr:1_{FBD00729-955E-40BC-9988-F120B241688E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{489D7849-9F73-4340-A142-C1F15B16DEE7}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D33D8996-AC77-49DD-81B7-1785A371AC8A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{4E765AEB-AA96-4461-9219-1D1C1A5882E1}"/>
+    <workbookView xWindow="-98" yWindow="16103" windowWidth="28996" windowHeight="15675" activeTab="1" xr2:uid="{4E765AEB-AA96-4461-9219-1D1C1A5882E1}"/>
   </bookViews>
   <sheets>
     <sheet name="Loadings" sheetId="3" r:id="rId1"/>
@@ -298,7 +298,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -321,13 +321,22 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="48">
+  <cellXfs count="51">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -457,6 +466,15 @@
     </xf>
     <xf numFmtId="1" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="16" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="16" fillId="3" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -480,10 +498,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -783,29 +797,30 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B7214EDA-22E6-4C33-8129-2E66563FCEC8}">
-  <dimension ref="A1:J19"/>
+  <dimension ref="A1:K19"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E40" sqref="E40"/>
+      <selection activeCell="K6" sqref="K6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.83203125" defaultRowHeight="14"/>
+  <sheetFormatPr defaultColWidth="8.8125" defaultRowHeight="13.5"/>
   <cols>
     <col min="1" max="1" width="10" customWidth="1"/>
-    <col min="2" max="2" width="9.33203125" customWidth="1"/>
-    <col min="3" max="3" width="9.6640625" customWidth="1"/>
+    <col min="2" max="2" width="9.3125" customWidth="1"/>
+    <col min="3" max="3" width="9.6875" customWidth="1"/>
     <col min="4" max="4" width="9.5" customWidth="1"/>
-    <col min="7" max="7" width="9.1640625" customWidth="1"/>
-    <col min="8" max="8" width="10.83203125" customWidth="1"/>
+    <col min="7" max="7" width="9.1875" customWidth="1"/>
+    <col min="8" max="8" width="10.8125" customWidth="1"/>
     <col min="9" max="9" width="10" customWidth="1"/>
+    <col min="10" max="10" width="8.8125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="15.5">
+    <row r="1" spans="1:11" ht="15">
       <c r="A1" s="29" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="3" spans="1:10" ht="15.5">
+    <row r="3" spans="1:11" ht="15.75">
       <c r="A3" s="17" t="s">
         <v>21</v>
       </c>
@@ -820,7 +835,7 @@
       <c r="H3" s="20"/>
       <c r="I3" s="20"/>
     </row>
-    <row r="4" spans="1:10" ht="15.5">
+    <row r="4" spans="1:11" ht="15">
       <c r="A4" s="21" t="s">
         <v>10</v>
       </c>
@@ -837,8 +852,9 @@
       </c>
       <c r="H4" s="22"/>
       <c r="I4" s="22"/>
-    </row>
-    <row r="5" spans="1:10" ht="15.5">
+      <c r="K4" s="48"/>
+    </row>
+    <row r="5" spans="1:11" ht="15">
       <c r="A5" s="23"/>
       <c r="B5" s="24"/>
       <c r="C5" s="25"/>
@@ -847,8 +863,9 @@
       <c r="G5" s="24"/>
       <c r="H5" s="25"/>
       <c r="I5" s="25"/>
-    </row>
-    <row r="6" spans="1:10" ht="15.5">
+      <c r="K5" s="48"/>
+    </row>
+    <row r="6" spans="1:11" ht="15">
       <c r="A6" s="23" t="s">
         <v>11</v>
       </c>
@@ -874,8 +891,9 @@
       <c r="I6" s="24" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="7" spans="1:10" ht="15.5">
+      <c r="K6" s="48"/>
+    </row>
+    <row r="7" spans="1:11" ht="15">
       <c r="A7" s="23">
         <v>1</v>
       </c>
@@ -889,8 +907,11 @@
       <c r="G7" s="24"/>
       <c r="H7" s="24"/>
       <c r="I7" s="25"/>
-    </row>
-    <row r="8" spans="1:10" ht="15.5">
+      <c r="K7" s="48">
+        <v>7.87</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" ht="15">
       <c r="A8" s="23">
         <v>2</v>
       </c>
@@ -904,8 +925,11 @@
       <c r="G8" s="27"/>
       <c r="H8" s="27"/>
       <c r="I8" s="27"/>
-    </row>
-    <row r="9" spans="1:10" ht="15.5">
+      <c r="K8" s="48">
+        <v>8.61</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" ht="15">
       <c r="A9" s="23">
         <v>3</v>
       </c>
@@ -926,8 +950,11 @@
         <v>85</v>
       </c>
       <c r="J9" s="35"/>
-    </row>
-    <row r="10" spans="1:10" ht="15.5">
+      <c r="K9" s="48">
+        <v>9.34</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" ht="15">
       <c r="A10" s="23">
         <v>4</v>
       </c>
@@ -953,8 +980,11 @@
         <v>82</v>
       </c>
       <c r="J10" s="35"/>
-    </row>
-    <row r="11" spans="1:10" ht="15.5">
+      <c r="K10" s="49">
+        <v>10.08</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" ht="15.75">
       <c r="A11" s="23">
         <v>5</v>
       </c>
@@ -980,8 +1010,11 @@
         <v>79</v>
       </c>
       <c r="J11" s="35"/>
-    </row>
-    <row r="12" spans="1:10" ht="15.5">
+      <c r="K11" s="48">
+        <v>10.82</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" ht="15.75">
       <c r="A12" s="23">
         <v>6</v>
       </c>
@@ -1007,8 +1040,11 @@
         <v>76</v>
       </c>
       <c r="J12" s="35"/>
-    </row>
-    <row r="13" spans="1:10" ht="15.5">
+      <c r="K12" s="48">
+        <v>11.73</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" ht="15.75">
       <c r="A13" s="23">
         <v>7</v>
       </c>
@@ -1034,8 +1070,11 @@
         <v>70</v>
       </c>
       <c r="J13" s="35"/>
-    </row>
-    <row r="14" spans="1:10" ht="15.5">
+      <c r="K13" s="48">
+        <v>12.49</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" ht="15.75">
       <c r="A14" s="23">
         <v>8</v>
       </c>
@@ -1061,8 +1100,11 @@
         <v>65</v>
       </c>
       <c r="J14" s="35"/>
-    </row>
-    <row r="15" spans="1:10" ht="15.5">
+      <c r="K14" s="48">
+        <v>13.23</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" ht="15.75">
       <c r="A15" s="23">
         <v>9</v>
       </c>
@@ -1088,8 +1130,11 @@
         <v>60</v>
       </c>
       <c r="J15" s="35"/>
-    </row>
-    <row r="16" spans="1:10" ht="15.5">
+      <c r="K15" s="50">
+        <v>13.96</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" ht="15.75">
       <c r="A16" s="23">
         <v>10</v>
       </c>
@@ -1115,8 +1160,11 @@
         <v>53</v>
       </c>
       <c r="J16" s="35"/>
-    </row>
-    <row r="17" spans="1:10" ht="15.5">
+      <c r="K16" s="50">
+        <v>14.7</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" ht="15.75">
       <c r="A17" s="23">
         <v>11</v>
       </c>
@@ -1136,8 +1184,11 @@
       <c r="H17" s="30"/>
       <c r="I17" s="30"/>
       <c r="J17" s="35"/>
-    </row>
-    <row r="18" spans="1:10" ht="15.5">
+      <c r="K17" s="48">
+        <v>15.49</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" ht="15">
       <c r="A18" s="21" t="s">
         <v>20</v>
       </c>
@@ -1156,7 +1207,7 @@
       <c r="I18" s="32"/>
       <c r="J18" s="35"/>
     </row>
-    <row r="19" spans="1:10">
+    <row r="19" spans="1:11">
       <c r="G19" s="35"/>
       <c r="H19" s="35"/>
       <c r="I19" s="35"/>
@@ -1171,40 +1222,40 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E300A503-FEA7-4473-B0E4-AD198B9D0951}">
   <dimension ref="A2:AI48"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="K14" sqref="K14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="14"/>
+  <sheetFormatPr defaultColWidth="8.6875" defaultRowHeight="13.5"/>
   <cols>
-    <col min="1" max="1" width="14.9140625" style="3" customWidth="1"/>
+    <col min="1" max="1" width="14.9375" style="3" customWidth="1"/>
     <col min="2" max="2" width="15.25" style="3" customWidth="1"/>
-    <col min="3" max="3" width="14.83203125" style="3" customWidth="1"/>
-    <col min="4" max="4" width="11.33203125" style="3" customWidth="1"/>
-    <col min="5" max="5" width="10.6640625" style="3" customWidth="1"/>
-    <col min="6" max="6" width="9.83203125" style="3" customWidth="1"/>
-    <col min="7" max="8" width="8.6640625" style="3"/>
-    <col min="9" max="9" width="14.6640625" style="3" customWidth="1"/>
-    <col min="10" max="10" width="14.33203125" style="3" customWidth="1"/>
-    <col min="11" max="11" width="16.08203125" style="3" customWidth="1"/>
-    <col min="12" max="12" width="11.1640625" style="3" customWidth="1"/>
-    <col min="13" max="13" width="10.33203125" style="3" customWidth="1"/>
-    <col min="14" max="15" width="8.6640625" style="3"/>
-    <col min="17" max="17" width="10.1640625" customWidth="1"/>
-    <col min="18" max="20" width="8.6640625" style="3"/>
-    <col min="24" max="29" width="8.6640625" style="3"/>
-    <col min="31" max="31" width="10.6640625" customWidth="1"/>
+    <col min="3" max="3" width="14.8125" style="3" customWidth="1"/>
+    <col min="4" max="4" width="11.3125" style="3" customWidth="1"/>
+    <col min="5" max="5" width="10.6875" style="3" customWidth="1"/>
+    <col min="6" max="6" width="9.8125" style="3" customWidth="1"/>
+    <col min="7" max="8" width="8.6875" style="3"/>
+    <col min="9" max="9" width="14.6875" style="3" customWidth="1"/>
+    <col min="10" max="10" width="14.3125" style="3" customWidth="1"/>
+    <col min="11" max="11" width="16.0625" style="3" customWidth="1"/>
+    <col min="12" max="12" width="11.1875" style="3" customWidth="1"/>
+    <col min="13" max="13" width="10.3125" style="3" customWidth="1"/>
+    <col min="14" max="15" width="8.6875" style="3"/>
+    <col min="17" max="17" width="10.1875" customWidth="1"/>
+    <col min="18" max="20" width="8.6875" style="3"/>
+    <col min="24" max="29" width="8.6875" style="3"/>
+    <col min="31" max="31" width="10.6875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:35">
+    <row r="2" spans="1:35" ht="13.9">
       <c r="A2" s="28" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="3" spans="1:35">
+    <row r="3" spans="1:35" ht="13.9">
       <c r="A3" s="14"/>
     </row>
-    <row r="4" spans="1:35">
+    <row r="4" spans="1:35" ht="13.9">
       <c r="A4" s="1" t="s">
         <v>0</v>
       </c>
@@ -1224,14 +1275,14 @@
       <c r="M4"/>
       <c r="N4"/>
     </row>
-    <row r="5" spans="1:35">
+    <row r="5" spans="1:35" ht="13.9">
       <c r="C5" s="4"/>
       <c r="D5" s="2"/>
       <c r="K5" s="4"/>
       <c r="M5"/>
       <c r="N5"/>
     </row>
-    <row r="6" spans="1:35">
+    <row r="6" spans="1:35" ht="13.9">
       <c r="A6" s="2" t="s">
         <v>3</v>
       </c>
@@ -1285,7 +1336,7 @@
       <c r="M7" s="6"/>
       <c r="N7" s="7"/>
     </row>
-    <row r="8" spans="1:35">
+    <row r="8" spans="1:35" ht="13.9">
       <c r="A8" s="44">
         <v>170.78120000000001</v>
       </c>
@@ -1314,7 +1365,7 @@
       <c r="AG8" s="3"/>
       <c r="AH8" s="2"/>
     </row>
-    <row r="9" spans="1:35">
+    <row r="9" spans="1:35" ht="13.9">
       <c r="A9" s="44">
         <v>160.48439999999999</v>
       </c>
@@ -1343,7 +1394,7 @@
       <c r="AG9" s="3"/>
       <c r="AH9" s="2"/>
     </row>
-    <row r="10" spans="1:35">
+    <row r="10" spans="1:35" ht="13.9">
       <c r="A10" s="44">
         <v>190.59370000000001</v>
       </c>
@@ -1403,7 +1454,7 @@
       <c r="AH11" s="3"/>
       <c r="AI11" s="9"/>
     </row>
-    <row r="12" spans="1:35">
+    <row r="12" spans="1:35" ht="13.9">
       <c r="C12" s="10" t="s">
         <v>31</v>
       </c>
@@ -1424,7 +1475,7 @@
       <c r="AH12" s="3"/>
       <c r="AI12" s="9"/>
     </row>
-    <row r="13" spans="1:35">
+    <row r="13" spans="1:35" ht="13.9">
       <c r="A13" s="44"/>
       <c r="B13" s="44"/>
       <c r="C13" s="44"/>
@@ -1440,7 +1491,7 @@
       <c r="AH13" s="3"/>
       <c r="AI13" s="9"/>
     </row>
-    <row r="14" spans="1:35">
+    <row r="14" spans="1:35" ht="13.9">
       <c r="D14" s="1"/>
       <c r="E14" s="13"/>
       <c r="I14"/>
@@ -1453,7 +1504,7 @@
       <c r="AH14" s="3"/>
       <c r="AI14" s="9"/>
     </row>
-    <row r="15" spans="1:35">
+    <row r="15" spans="1:35" ht="13.9">
       <c r="A15" s="28" t="s">
         <v>16</v>
       </c>
@@ -1465,7 +1516,7 @@
       <c r="AH15" s="3"/>
       <c r="AI15" s="9"/>
     </row>
-    <row r="16" spans="1:35">
+    <row r="16" spans="1:35" ht="13.9">
       <c r="A16" s="14"/>
       <c r="D16" s="2"/>
       <c r="E16" s="12"/>
@@ -1475,7 +1526,7 @@
       <c r="AH16" s="3"/>
       <c r="AI16" s="9"/>
     </row>
-    <row r="17" spans="1:35">
+    <row r="17" spans="1:35" ht="13.9">
       <c r="A17" s="1" t="s">
         <v>4</v>
       </c>
@@ -1500,7 +1551,7 @@
       <c r="AH17" s="3"/>
       <c r="AI17" s="9"/>
     </row>
-    <row r="18" spans="1:35">
+    <row r="18" spans="1:35" ht="13.9">
       <c r="A18" s="2" t="s">
         <v>5</v>
       </c>
@@ -1521,7 +1572,7 @@
       <c r="AH18" s="11"/>
       <c r="AI18" s="3"/>
     </row>
-    <row r="19" spans="1:35">
+    <row r="19" spans="1:35" ht="14.25">
       <c r="A19" s="2" t="s">
         <v>28</v>
       </c>
@@ -1556,7 +1607,7 @@
       <c r="AG19" s="1"/>
       <c r="AH19" s="13"/>
     </row>
-    <row r="20" spans="1:35">
+    <row r="20" spans="1:35" ht="13.9">
       <c r="A20" s="8">
         <v>0.20255000000000001</v>
       </c>
@@ -1588,7 +1639,7 @@
       <c r="AE20" s="2"/>
       <c r="AF20" s="3"/>
     </row>
-    <row r="21" spans="1:35">
+    <row r="21" spans="1:35" ht="13.9">
       <c r="A21" s="8">
         <v>-0.68074999999999997</v>
       </c>
@@ -1620,7 +1671,7 @@
       <c r="AE21" s="2"/>
       <c r="AF21" s="3"/>
     </row>
-    <row r="22" spans="1:35">
+    <row r="22" spans="1:35" ht="13.9">
       <c r="A22" s="8">
         <v>-1.1865999999999999</v>
       </c>
@@ -1652,7 +1703,7 @@
       <c r="AE22" s="2"/>
       <c r="AF22" s="3"/>
     </row>
-    <row r="23" spans="1:35">
+    <row r="23" spans="1:35" ht="13.9">
       <c r="A23" s="8">
         <v>-2.9811999999999999</v>
       </c>
@@ -1714,7 +1765,7 @@
       <c r="AE24" s="3"/>
       <c r="AF24" s="3"/>
     </row>
-    <row r="25" spans="1:35">
+    <row r="25" spans="1:35" ht="13.9">
       <c r="A25" s="43"/>
       <c r="B25" s="43"/>
       <c r="C25" s="10" t="s">
@@ -1741,7 +1792,7 @@
       <c r="AF25" s="3"/>
       <c r="AG25" s="16"/>
     </row>
-    <row r="26" spans="1:35">
+    <row r="26" spans="1:35" ht="13.9">
       <c r="A26" s="45"/>
       <c r="B26" s="35"/>
       <c r="C26" s="45"/>
@@ -1761,7 +1812,7 @@
       <c r="AF26" s="3"/>
       <c r="AG26" s="16"/>
     </row>
-    <row r="28" spans="1:35">
+    <row r="28" spans="1:35" ht="13.9">
       <c r="A28" s="14" t="s">
         <v>17</v>
       </c>
@@ -1769,7 +1820,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="29" spans="1:35">
+    <row r="29" spans="1:35" ht="13.9">
       <c r="A29" s="1" t="s">
         <v>1</v>
       </c>
@@ -1789,7 +1840,7 @@
       <c r="M29" s="5"/>
       <c r="N29" s="5"/>
     </row>
-    <row r="31" spans="1:35">
+    <row r="31" spans="1:35" ht="13.9">
       <c r="A31" s="2" t="s">
         <v>25</v>
       </c>
@@ -2051,6 +2102,77 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<spe:Receivers xmlns:spe="http://schemas.microsoft.com/sharepoint/events">
+  <Receiver>
+    <Name>Document ID Generator</Name>
+    <Synchronization>Synchronous</Synchronization>
+    <Type>10001</Type>
+    <SequenceNumber>1000</SequenceNumber>
+    <Url/>
+    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
+    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
+    <Data/>
+    <Filter/>
+  </Receiver>
+  <Receiver>
+    <Name>Document ID Generator</Name>
+    <Synchronization>Synchronous</Synchronization>
+    <Type>10002</Type>
+    <SequenceNumber>1001</SequenceNumber>
+    <Url/>
+    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
+    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
+    <Data/>
+    <Filter/>
+  </Receiver>
+  <Receiver>
+    <Name>Document ID Generator</Name>
+    <Synchronization>Synchronous</Synchronization>
+    <Type>10004</Type>
+    <SequenceNumber>1002</SequenceNumber>
+    <Url/>
+    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
+    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
+    <Data/>
+    <Filter/>
+  </Receiver>
+  <Receiver>
+    <Name>Document ID Generator</Name>
+    <Synchronization>Synchronous</Synchronization>
+    <Type>10006</Type>
+    <SequenceNumber>1003</SequenceNumber>
+    <Url/>
+    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
+    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
+    <Data/>
+    <Filter/>
+  </Receiver>
+</spe:Receivers>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_dlc_DocId xmlns="5e91c50e-ace1-45b7-a3e6-97bcf1bdb737">T535JUCYK326-1424725285-25657</_dlc_DocId>
+    <_dlc_DocIdUrl xmlns="5e91c50e-ace1-45b7-a3e6-97bcf1bdb737">
+      <Url>https://cranfield.sharepoint.com/sites/SATMShare/_layouts/15/DocIdRedir.aspx?ID=T535JUCYK326-1424725285-25657</Url>
+      <Description>T535JUCYK326-1424725285-25657</Description>
+    </_dlc_DocIdUrl>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100EE62243AC7650B47BAC141A22364FD77" ma:contentTypeVersion="38064" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="f711a72f3b470c00b8a37d4f23966a3d">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="5e91c50e-ace1-45b7-a3e6-97bcf1bdb737" xmlns:ns3="2559487d-57cf-4208-80b0-50671af47a2d" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="008c37ebe60ab966e5f28b1c3e1cc6a0" ns2:_="" ns3:_="">
     <xsd:import namespace="5e91c50e-ace1-45b7-a3e6-97bcf1bdb737"/>
@@ -2298,78 +2420,33 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_dlc_DocId xmlns="5e91c50e-ace1-45b7-a3e6-97bcf1bdb737">T535JUCYK326-1424725285-25657</_dlc_DocId>
-    <_dlc_DocIdUrl xmlns="5e91c50e-ace1-45b7-a3e6-97bcf1bdb737">
-      <Url>https://cranfield.sharepoint.com/sites/SATMShare/_layouts/15/DocIdRedir.aspx?ID=T535JUCYK326-1424725285-25657</Url>
-      <Description>T535JUCYK326-1424725285-25657</Description>
-    </_dlc_DocIdUrl>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{23E1CD13-EE80-43A8-B0D3-2175FDEBB3E0}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/events"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FAA0AD98-B848-4C41-8E5E-A5B257945FA8}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<spe:Receivers xmlns:spe="http://schemas.microsoft.com/sharepoint/events">
-  <Receiver>
-    <Name>Document ID Generator</Name>
-    <Synchronization>Synchronous</Synchronization>
-    <Type>10001</Type>
-    <SequenceNumber>1000</SequenceNumber>
-    <Url/>
-    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
-    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
-    <Data/>
-    <Filter/>
-  </Receiver>
-  <Receiver>
-    <Name>Document ID Generator</Name>
-    <Synchronization>Synchronous</Synchronization>
-    <Type>10002</Type>
-    <SequenceNumber>1001</SequenceNumber>
-    <Url/>
-    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
-    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
-    <Data/>
-    <Filter/>
-  </Receiver>
-  <Receiver>
-    <Name>Document ID Generator</Name>
-    <Synchronization>Synchronous</Synchronization>
-    <Type>10004</Type>
-    <SequenceNumber>1002</SequenceNumber>
-    <Url/>
-    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
-    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
-    <Data/>
-    <Filter/>
-  </Receiver>
-  <Receiver>
-    <Name>Document ID Generator</Name>
-    <Synchronization>Synchronous</Synchronization>
-    <Type>10006</Type>
-    <SequenceNumber>1003</SequenceNumber>
-    <Url/>
-    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
-    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
-    <Data/>
-    <Filter/>
-  </Receiver>
-</spe:Receivers>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F279BDFF-E2A3-40C7-BAC4-6506C5AB7C1A}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="5e91c50e-ace1-45b7-a3e6-97bcf1bdb737"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{818E3C31-C35F-46F9-B619-6D7A4BE0047A}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2386,30 +2463,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F279BDFF-E2A3-40C7-BAC4-6506C5AB7C1A}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="5e91c50e-ace1-45b7-a3e6-97bcf1bdb737"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FAA0AD98-B848-4C41-8E5E-A5B257945FA8}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{23E1CD13-EE80-43A8-B0D3-2175FDEBB3E0}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/events"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>